<commit_message>
changed the aabsolute xpaths to relative xpaths
</commit_message>
<xml_diff>
--- a/DataEngine.xlsx
+++ b/DataEngine.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venkata\Downloads\NapierHeathCareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{E81D89B7-8711-449C-AE9A-8AEB4A787253}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C785F5-9548-4EE9-8AA4-78A0E008D813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{0CBD72DD-247D-49CC-8DC1-EA3478D72631}" yWindow="-108"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CBD72DD-247D-49CC-8DC1-EA3478D72631}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" r:id="rId1" sheetId="1"/>
-    <sheet name="LoginData" r:id="rId2" sheetId="3"/>
-    <sheet name="TC_IncidentReport" r:id="rId3" sheetId="4"/>
-    <sheet name="TC_IncidentReportAllDetails" r:id="rId4" sheetId="5"/>
-    <sheet name="TC_IncidentReportSaveSubmit" r:id="rId5" sheetId="6"/>
-    <sheet name="TC_IncidentReportAnonymouslyAll" r:id="rId6" sheetId="7"/>
-    <sheet name="TC_InciRepPatientComplaint" r:id="rId7" sheetId="8"/>
-    <sheet name="TC_QualityDashboardAssign" r:id="rId8" sheetId="9"/>
-    <sheet name="TC_QualityDashboardReAssign" r:id="rId9" sheetId="10"/>
+    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="3" r:id="rId2"/>
+    <sheet name="TC_IncidentReport" sheetId="4" r:id="rId3"/>
+    <sheet name="TC_IncidentReportAllDetails" sheetId="5" r:id="rId4"/>
+    <sheet name="TC_IncidentReportSaveSubmit" sheetId="6" r:id="rId5"/>
+    <sheet name="TC_IncidentReportAnonymouslyAll" sheetId="7" r:id="rId6"/>
+    <sheet name="TC_InciRepPatientComplaint" sheetId="8" r:id="rId7"/>
+    <sheet name="TC_QualityDashboardAssign" sheetId="9" r:id="rId8"/>
+    <sheet name="TC_QualityDashboardReAssign" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="83">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -289,21 +289,16 @@
 IR Code: 318 /2022 CONFIG CODE</t>
   </si>
   <si>
-    <t>315 /2022 CONFIG CODE</t>
-  </si>
-  <si>
-    <t>Incident was successfully Submitted.
-IR Code: 321 /2022 CONFIG CODE</t>
-  </si>
-  <si>
-    <t>324 /2022 CONFIG CODE</t>
+    <t>325 /2022 CONFIG CODE</t>
+  </si>
+  <si>
+    <t>326 /2022 CONFIG CODE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -375,34 +370,34 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -419,10 +414,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -457,7 +452,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -509,7 +504,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -620,21 +615,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -651,7 +646,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -703,25 +698,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF4FBAF-171D-453E-AB44-6EDA8B53361F}">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF4FBAF-171D-453E-AB44-6EDA8B53361F}">
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="69.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="69.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -743,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -908,7 +903,7 @@
         <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -919,7 +914,7 @@
         <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -930,7 +925,7 @@
         <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -941,7 +936,7 @@
         <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -952,7 +947,7 @@
         <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -963,18 +958,18 @@
         <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4467D1C-6514-4B86-BE3A-23BA116DD8A8}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4467D1C-6514-4B86-BE3A-23BA116DD8A8}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -982,9 +977,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="17.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="17.44140625" collapsed="true"/>
-    <col min="3" max="16384" style="2" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="17.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1013,17 +1008,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{D016C0B6-99AF-401B-BF94-CB5BAA361BDA}"/>
-    <hyperlink r:id="rId2" ref="B3" xr:uid="{0EA09625-7286-4381-BBD8-70D12B6B7045}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D016C0B6-99AF-401B-BF94-CB5BAA361BDA}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{0EA09625-7286-4381-BBD8-70D12B6B7045}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F648FE-926A-4AF0-9192-B08639DEAB9D}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F648FE-926A-4AF0-9192-B08639DEAB9D}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -1031,13 +1026,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1063,7 +1058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1083,32 +1078,32 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DE333-4886-4A33-96E8-FE088607B0BE}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DE333-4886-4A33-96E8-FE088607B0BE}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="7" max="14" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="14" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1158,7 +1153,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1206,13 +1201,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C8E9E0-5EE2-47D8-9BD1-DD56248288CF}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C8E9E0-5EE2-47D8-9BD1-DD56248288CF}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -1220,13 +1215,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1252,7 +1247,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1276,28 +1271,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8504A7C3-CF4C-4515-8156-88A57D587F8A}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8504A7C3-CF4C-4515-8156-88A57D587F8A}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="7" max="13" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="13" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1344,7 +1339,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1389,13 +1384,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C479C5-F6DE-4AAF-BAEC-85BD0B03C9C6}">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C479C5-F6DE-4AAF-BAEC-85BD0B03C9C6}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
@@ -1403,14 +1398,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="9" max="15" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="15" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -1463,7 +1458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1512,14 +1507,14 @@
       <c r="P2" s="8"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6500C3B1-9DA3-4401-AFFF-7A1389B64A9F}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6500C3B1-9DA3-4401-AFFF-7A1389B64A9F}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1527,8 +1522,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1541,30 +1536,30 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84899ADB-4152-4A35-A75F-377100608B27}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84899ADB-4152-4A35-A75F-377100608B27}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1577,13 +1572,13 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified patient complaint test case
</commit_message>
<xml_diff>
--- a/DataEngine.xlsx
+++ b/DataEngine.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venkata\Downloads\NapierHeathCareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C785F5-9548-4EE9-8AA4-78A0E008D813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{DE945D75-1B2F-44FC-8447-BBEFB688ED9B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CBD72DD-247D-49CC-8DC1-EA3478D72631}"/>
+    <workbookView activeTab="6" firstSheet="4" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{0CBD72DD-247D-49CC-8DC1-EA3478D72631}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginData" sheetId="3" r:id="rId2"/>
-    <sheet name="TC_IncidentReport" sheetId="4" r:id="rId3"/>
-    <sheet name="TC_IncidentReportAllDetails" sheetId="5" r:id="rId4"/>
-    <sheet name="TC_IncidentReportSaveSubmit" sheetId="6" r:id="rId5"/>
-    <sheet name="TC_IncidentReportAnonymouslyAll" sheetId="7" r:id="rId6"/>
-    <sheet name="TC_InciRepPatientComplaint" sheetId="8" r:id="rId7"/>
-    <sheet name="TC_QualityDashboardAssign" sheetId="9" r:id="rId8"/>
-    <sheet name="TC_QualityDashboardReAssign" sheetId="10" r:id="rId9"/>
+    <sheet name="Test Cases" r:id="rId1" sheetId="1"/>
+    <sheet name="LoginData" r:id="rId2" sheetId="3"/>
+    <sheet name="TC_IncidentReport" r:id="rId3" sheetId="4"/>
+    <sheet name="TC_IncidentReportAllDetails" r:id="rId4" sheetId="5"/>
+    <sheet name="TC_IncidentReportSaveSubmit" r:id="rId5" sheetId="6"/>
+    <sheet name="TC_IncidentReportAnonymouslyAll" r:id="rId6" sheetId="7"/>
+    <sheet name="TC_InciRepPatientComplaint" r:id="rId7" sheetId="8"/>
+    <sheet name="TC_QualityDashboardAssign" r:id="rId8" sheetId="9"/>
+    <sheet name="TC_QualityDashboardReAssign" r:id="rId9" sheetId="10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="90">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -282,10 +282,6 @@
   </si>
   <si>
     <t>Incident was successfully Submitted.
-IR Code: 316 /2022 CONFIG CODE</t>
-  </si>
-  <si>
-    <t>Incident was successfully Submitted.
 IR Code: 318 /2022 CONFIG CODE</t>
   </si>
   <si>
@@ -293,12 +289,37 @@
   </si>
   <si>
     <t>326 /2022 CONFIG CODE</t>
+  </si>
+  <si>
+    <t>344 /2022 CONFIG CODE</t>
+  </si>
+  <si>
+    <t>Patient Name</t>
+  </si>
+  <si>
+    <t>Mr. Fashish</t>
+  </si>
+  <si>
+    <t>Clinical</t>
+  </si>
+  <si>
+    <t>Billing</t>
+  </si>
+  <si>
+    <t>Eric M Doc</t>
+  </si>
+  <si>
+    <t>Raghu M Doc</t>
+  </si>
+  <si>
+    <t>345 /2022 CONFIG CODE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -370,34 +391,34 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -414,10 +435,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -452,7 +473,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -504,7 +525,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -615,21 +636,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -646,7 +667,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -698,25 +719,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF4FBAF-171D-453E-AB44-6EDA8B53361F}">
-  <dimension ref="A1:C22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF4FBAF-171D-453E-AB44-6EDA8B53361F}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="69.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="69.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -738,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -782,7 +803,7 @@
         <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -962,14 +983,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4467D1C-6514-4B86-BE3A-23BA116DD8A8}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4467D1C-6514-4B86-BE3A-23BA116DD8A8}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -977,9 +998,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="8.88671875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="17.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="17.44140625" collapsed="true"/>
+    <col min="3" max="16384" style="2" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1008,17 +1029,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{D016C0B6-99AF-401B-BF94-CB5BAA361BDA}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{0EA09625-7286-4381-BBD8-70D12B6B7045}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{D016C0B6-99AF-401B-BF94-CB5BAA361BDA}"/>
+    <hyperlink r:id="rId2" ref="B3" xr:uid="{0EA09625-7286-4381-BBD8-70D12B6B7045}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F648FE-926A-4AF0-9192-B08639DEAB9D}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F648FE-926A-4AF0-9192-B08639DEAB9D}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -1026,13 +1047,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1058,7 +1079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1078,17 +1099,17 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DE333-4886-4A33-96E8-FE088607B0BE}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DE333-4886-4A33-96E8-FE088607B0BE}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
@@ -1096,14 +1117,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="14" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="7" max="14" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1153,7 +1174,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1197,17 +1218,17 @@
         <v>26</v>
       </c>
       <c r="O2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C8E9E0-5EE2-47D8-9BD1-DD56248288CF}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C8E9E0-5EE2-47D8-9BD1-DD56248288CF}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -1215,13 +1236,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1247,7 +1268,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1271,13 +1292,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8504A7C3-CF4C-4515-8156-88A57D587F8A}">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8504A7C3-CF4C-4515-8156-88A57D587F8A}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
@@ -1285,14 +1306,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="13" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="7" max="13" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="16.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1339,7 +1360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1380,35 +1401,37 @@
         <v>1102202118390</v>
       </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C479C5-F6DE-4AAF-BAEC-85BD0B03C9C6}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C479C5-F6DE-4AAF-BAEC-85BD0B03C9C6}">
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="15" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.109375" collapsed="false"/>
+    <col min="5" max="6" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="10" max="16" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="16.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -1419,102 +1442,108 @@
         <v>13</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="6">
         <v>1102202118390</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="J2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="6">
+      <c r="L2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="6">
         <v>1102202118390</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="N2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="6">
-        <v>1102202118390</v>
-      </c>
-      <c r="P2" s="8"/>
+        <v>87</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6500C3B1-9DA3-4401-AFFF-7A1389B64A9F}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6500C3B1-9DA3-4401-AFFF-7A1389B64A9F}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1522,8 +1551,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1536,21 +1565,21 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84899ADB-4152-4A35-A75F-377100608B27}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84899ADB-4152-4A35-A75F-377100608B27}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -1558,8 +1587,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1572,13 +1601,13 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added testcases for acknowledgement and turn around time
</commit_message>
<xml_diff>
--- a/DataEngine.xlsx
+++ b/DataEngine.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venkata\Downloads\NapierHeathCareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{DE945D75-1B2F-44FC-8447-BBEFB688ED9B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9858D4EA-281E-418E-8811-8171792B6292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="4" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{0CBD72DD-247D-49CC-8DC1-EA3478D72631}" yWindow="-108"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CBD72DD-247D-49CC-8DC1-EA3478D72631}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" r:id="rId1" sheetId="1"/>
-    <sheet name="LoginData" r:id="rId2" sheetId="3"/>
-    <sheet name="TC_IncidentReport" r:id="rId3" sheetId="4"/>
-    <sheet name="TC_IncidentReportAllDetails" r:id="rId4" sheetId="5"/>
-    <sheet name="TC_IncidentReportSaveSubmit" r:id="rId5" sheetId="6"/>
-    <sheet name="TC_IncidentReportAnonymouslyAll" r:id="rId6" sheetId="7"/>
-    <sheet name="TC_InciRepPatientComplaint" r:id="rId7" sheetId="8"/>
-    <sheet name="TC_QualityDashboardAssign" r:id="rId8" sheetId="9"/>
-    <sheet name="TC_QualityDashboardReAssign" r:id="rId9" sheetId="10"/>
+    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="3" r:id="rId2"/>
+    <sheet name="TC_IncidentReport" sheetId="4" r:id="rId3"/>
+    <sheet name="TC_IncidentReportAllDetails" sheetId="5" r:id="rId4"/>
+    <sheet name="TC_IncidentReportSaveSubmit" sheetId="6" r:id="rId5"/>
+    <sheet name="TC_IncidentReportAnonymouslyAll" sheetId="7" r:id="rId6"/>
+    <sheet name="TC_InciRepPatientComplaint" sheetId="8" r:id="rId7"/>
+    <sheet name="TC_QualityDashboardAssign" sheetId="9" r:id="rId8"/>
+    <sheet name="TC_QualityDashboardReAssign" sheetId="10" r:id="rId9"/>
+    <sheet name="TC_IR_TAT" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="98">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -313,13 +314,36 @@
   </si>
   <si>
     <t>345 /2022 CONFIG CODE</t>
+  </si>
+  <si>
+    <t>TC_IRinvestigationRecordInputs</t>
+  </si>
+  <si>
+    <t>TC_IRinvestigation</t>
+  </si>
+  <si>
+    <t>TC_IR_TAT</t>
+  </si>
+  <si>
+    <t>Tests the investigation functionality with asking details</t>
+  </si>
+  <si>
+    <t>Tests the investigation functionality with filling details</t>
+  </si>
+  <si>
+    <t>Tests the acknowledge functionality of the incidents</t>
+  </si>
+  <si>
+    <t>Tests the Turn Around Time functionality of the incidents</t>
+  </si>
+  <si>
+    <t>TC_IRAcknowledge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,34 +415,40 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -435,10 +465,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -473,7 +503,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -525,7 +555,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -636,21 +666,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -667,7 +697,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -719,25 +749,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF4FBAF-171D-453E-AB44-6EDA8B53361F}">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF4FBAF-171D-453E-AB44-6EDA8B53361F}">
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="69.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="69.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -803,7 +833,7 @@
         <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -982,15 +1012,87 @@
         <v>78</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26C12C4-C1BB-4B79-B73F-431C60FE2995}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4467D1C-6514-4B86-BE3A-23BA116DD8A8}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4467D1C-6514-4B86-BE3A-23BA116DD8A8}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -998,9 +1100,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="17.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="17.44140625" collapsed="true"/>
-    <col min="3" max="16384" style="2" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="17.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1029,17 +1131,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{D016C0B6-99AF-401B-BF94-CB5BAA361BDA}"/>
-    <hyperlink r:id="rId2" ref="B3" xr:uid="{0EA09625-7286-4381-BBD8-70D12B6B7045}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D016C0B6-99AF-401B-BF94-CB5BAA361BDA}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{0EA09625-7286-4381-BBD8-70D12B6B7045}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F648FE-926A-4AF0-9192-B08639DEAB9D}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F648FE-926A-4AF0-9192-B08639DEAB9D}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -1047,13 +1149,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1079,7 +1181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1103,13 +1205,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DE333-4886-4A33-96E8-FE088607B0BE}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DE333-4886-4A33-96E8-FE088607B0BE}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
@@ -1117,14 +1219,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="7" max="14" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="14" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1174,7 +1276,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1222,13 +1324,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C8E9E0-5EE2-47D8-9BD1-DD56248288CF}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C8E9E0-5EE2-47D8-9BD1-DD56248288CF}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -1236,13 +1338,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1268,7 +1370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1292,13 +1394,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8504A7C3-CF4C-4515-8156-88A57D587F8A}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8504A7C3-CF4C-4515-8156-88A57D587F8A}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
@@ -1306,14 +1408,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="7" max="13" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="13" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1360,7 +1462,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1405,30 +1507,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C479C5-F6DE-4AAF-BAEC-85BD0B03C9C6}">
-  <dimension ref="A1:R2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C479C5-F6DE-4AAF-BAEC-85BD0B03C9C6}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.109375" collapsed="false"/>
-    <col min="5" max="6" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="10" max="16" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="6" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="16" width="19.109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -1484,7 +1586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1102202118390</v>
       </c>
@@ -1536,14 +1638,14 @@
       <c r="Q2" s="8"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6500C3B1-9DA3-4401-AFFF-7A1389B64A9F}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6500C3B1-9DA3-4401-AFFF-7A1389B64A9F}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1551,8 +1653,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1572,23 +1674,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84899ADB-4152-4A35-A75F-377100608B27}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84899ADB-4152-4A35-A75F-377100608B27}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1608,6 +1710,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes in reporting for pass.
</commit_message>
<xml_diff>
--- a/DataEngine.xlsx
+++ b/DataEngine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venkata\Downloads\NapierHeathCareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9858D4EA-281E-418E-8811-8171792B6292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7828D418-7EAA-4BEA-AEBD-CBF197A5762C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CBD72DD-247D-49CC-8DC1-EA3478D72631}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="TC_InciRepPatientComplaint" sheetId="8" r:id="rId7"/>
     <sheet name="TC_QualityDashboardAssign" sheetId="9" r:id="rId8"/>
     <sheet name="TC_QualityDashboardReAssign" sheetId="10" r:id="rId9"/>
-    <sheet name="TC_IR_TAT" sheetId="11" r:id="rId10"/>
+    <sheet name="TC_IRAcknowledge" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="99">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>TC_IRAcknowledge</t>
+  </si>
+  <si>
+    <t>009 /06/2022 NAP H</t>
   </si>
 </sst>
 </file>
@@ -760,7 +763,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,7 +1070,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1082,7 +1085,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing 3 new Test cases: TC_IRinvestigationRequestInput, TC_IRinvestigationRecordInputs, TC_IRinvestigationIRDetails
</commit_message>
<xml_diff>
--- a/DataEngine.xlsx
+++ b/DataEngine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venkata\Downloads\NapierHeathCareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7828D418-7EAA-4BEA-AEBD-CBF197A5762C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7548D8-A673-4F21-85DC-91E0D4A40DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CBD72DD-247D-49CC-8DC1-EA3478D72631}"/>
   </bookViews>
@@ -23,6 +23,9 @@
     <sheet name="TC_QualityDashboardAssign" sheetId="9" r:id="rId8"/>
     <sheet name="TC_QualityDashboardReAssign" sheetId="10" r:id="rId9"/>
     <sheet name="TC_IRAcknowledge" sheetId="11" r:id="rId10"/>
+    <sheet name="TC_IRinvestigationRequestInput" sheetId="12" r:id="rId11"/>
+    <sheet name="TC_IRinvestigationRecordInputs" sheetId="13" r:id="rId12"/>
+    <sheet name="TC_IRinvestigationIRDetails" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="113">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -57,9 +60,6 @@
   </si>
   <si>
     <t>Tests the complete workflow of creating the incident.</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>username</t>
@@ -319,9 +319,6 @@
     <t>TC_IRinvestigationRecordInputs</t>
   </si>
   <si>
-    <t>TC_IRinvestigation</t>
-  </si>
-  <si>
     <t>TC_IR_TAT</t>
   </si>
   <si>
@@ -341,6 +338,54 @@
   </si>
   <si>
     <t>009 /06/2022 NAP H</t>
+  </si>
+  <si>
+    <t>TC_IRinvestigationRequestInput</t>
+  </si>
+  <si>
+    <t>TC_IRinvestigationIRDetails</t>
+  </si>
+  <si>
+    <t>018 /06/2022 NAP H</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>test query for automation</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>Test response from query dashboard</t>
+  </si>
+  <si>
+    <t>test response in Record inputs</t>
+  </si>
+  <si>
+    <t>EventDetails</t>
+  </si>
+  <si>
+    <t>auto test1</t>
+  </si>
+  <si>
+    <t>notesName</t>
+  </si>
+  <si>
+    <t>notesDetails</t>
+  </si>
+  <si>
+    <t>test1</t>
   </si>
 </sst>
 </file>
@@ -420,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,6 +491,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF4FBAF-171D-453E-AB44-6EDA8B53361F}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,238 +841,238 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
         <v>65</v>
       </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
         <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1034,7 +1083,7 @@
         <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1042,21 +1091,32 @@
         <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
         <v>92</v>
       </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1070,7 +1130,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,12 +1140,153 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A57E34-D58B-4304-920C-3F70589B0C72}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="33.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760331C4-47A6-4829-8D0B-4C78444B4E8F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5F0FFC-DAC0-43B4-98EE-057BC97E92AF}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1110,26 +1311,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1147,7 +1348,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,25 +1364,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1189,22 +1390,22 @@
         <v>1102202118390</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1234,49 +1435,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="O1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1284,46 +1485,46 @@
         <v>1102202118390</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="H2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="J2" s="6">
         <v>1102202118390</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M2" s="6">
         <v>1102202118390</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1352,25 +1553,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1378,22 +1579,22 @@
         <v>1102202118390</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="G2" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1423,46 +1624,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="N1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1470,43 +1671,43 @@
         <v>1102202118390</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="H2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="J2" s="6">
         <v>1102202118390</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M2" s="6">
         <v>1102202118390</v>
       </c>
       <c r="N2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1538,55 +1739,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="M1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="Q1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1594,49 +1795,49 @@
         <v>1102202118390</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E2" s="6">
         <v>1102202118390</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M2" s="6">
         <v>1102202118390</v>
       </c>
       <c r="N2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" t="s">
         <v>88</v>
-      </c>
-      <c r="P2" t="s">
-        <v>89</v>
       </c>
       <c r="Q2" s="8"/>
     </row>
@@ -1662,18 +1863,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1698,18 +1899,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added feedback for sprint5
</commit_message>
<xml_diff>
--- a/DataEngine.xlsx
+++ b/DataEngine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venkata\Downloads\NapierHeathCareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7548D8-A673-4F21-85DC-91E0D4A40DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B4EE8C-B1B1-4D80-838C-F39992060117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CBD72DD-247D-49CC-8DC1-EA3478D72631}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="122">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -386,6 +386,33 @@
   </si>
   <si>
     <t>test1</t>
+  </si>
+  <si>
+    <t>EditDetails</t>
+  </si>
+  <si>
+    <t>edited event</t>
+  </si>
+  <si>
+    <t>Risk ID</t>
+  </si>
+  <si>
+    <t>Evidence Description</t>
+  </si>
+  <si>
+    <t>edited query</t>
+  </si>
+  <si>
+    <t>edited query for automation</t>
+  </si>
+  <si>
+    <t>TC_IRinvestigationIRDetailsEditDelete</t>
+  </si>
+  <si>
+    <t>Tests the investigation functionality with filling details in IR details</t>
+  </si>
+  <si>
+    <t>Tests the edit and delete functionality in IR details</t>
   </si>
 </sst>
 </file>
@@ -809,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF4FBAF-171D-453E-AB44-6EDA8B53361F}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,7 +1121,7 @@
         <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1105,7 +1132,7 @@
         <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1113,9 +1140,20 @@
         <v>98</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1155,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A57E34-D58B-4304-920C-3F70589B0C72}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,9 +1206,10 @@
     <col min="3" max="3" width="16.109375" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
     <col min="5" max="5" width="33.88671875" customWidth="1"/>
+    <col min="6" max="6" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>43</v>
       </c>
@@ -1186,8 +1225,11 @@
       <c r="E1" s="13" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>99</v>
       </c>
@@ -1202,6 +1244,9 @@
       </c>
       <c r="E2" s="12" t="s">
         <v>106</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1212,31 +1257,38 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760331C4-47A6-4829-8D0B-4C78444B4E8F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>99</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1247,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5F0FFC-DAC0-43B4-98EE-057BC97E92AF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1259,9 +1311,11 @@
     <col min="2" max="2" width="14.109375" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>43</v>
       </c>
@@ -1274,8 +1328,14 @@
       <c r="D1" s="13" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>99</v>
       </c>
@@ -1287,6 +1347,12 @@
       </c>
       <c r="D2" s="12" t="s">
         <v>112</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="12">
+        <v>63839994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>